<commit_message>
Add A7 - A12
</commit_message>
<xml_diff>
--- a/Blockpower/evidence.xlsx
+++ b/Blockpower/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tiger/dev/GitHub/gon-evidence/Blockpower/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9F6240-C120-0F43-98FB-2E73D2413953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7576504C-6891-9543-8132-9DE760BA8A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26460" yWindow="7920" windowWidth="42960" windowHeight="15260" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27860" yWindow="4700" windowWidth="42960" windowHeight="15260" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="57">
   <si>
     <t>TeamName</t>
   </si>
@@ -82,15 +82,9 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>dest chain id</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
     <t>tx hash on that chain</t>
   </si>
   <si>
@@ -208,6 +202,43 @@
   <si>
     <t>852B88402ACB856C89977507543CE74F41866343313D47A493DDA3CE999785AF</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bptaska7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/6BE1FAFF3DEDC87A4981EFCF5667DEBDD736AB0E20F6968816DDE7D01D88B997</t>
+  </si>
+  <si>
+    <t>bptaska8</t>
+  </si>
+  <si>
+    <t>ibc/DCF8F49DCEED9C6CFC55BB4347196C53C36D149D07E045798A2D804E9E0E4B0F</t>
+  </si>
+  <si>
+    <t>bptaska9</t>
+  </si>
+  <si>
+    <t>ibc/E61DFB9DEBBDDA4E1FAD0A7E2E47F1099024EC0C729183FE62FBCA85D2F866B0</t>
+  </si>
+  <si>
+    <t>bptaska10</t>
+  </si>
+  <si>
+    <t>ibc/DC312459FCB431C0024BF318A0B98421DD75B026292C9589EDB7C0C6DFBAE086</t>
+  </si>
+  <si>
+    <t>bptask11</t>
+  </si>
+  <si>
+    <t>ibc/196CF8E19F258DF7AC7449DA0BF6B1CE368F2CA9D6D8563625CAAFF616F71C1C</t>
+  </si>
+  <si>
+    <t>bptaska12</t>
+  </si>
+  <si>
+    <t>ibc/493B6D2E64E680578A96F085CAEFBE2E23CDE183F58A242F43970EA0028DD201</t>
   </si>
 </sst>
 </file>
@@ -291,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -306,7 +337,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -658,25 +688,25 @@
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1">
       <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -692,7 +722,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
@@ -710,10 +742,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>50</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -729,7 +761,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
@@ -747,10 +781,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>52</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -766,7 +800,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
@@ -784,10 +820,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>54</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -803,7 +839,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
@@ -821,10 +859,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>56</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -858,20 +896,20 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -905,20 +943,20 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -952,20 +990,20 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -999,20 +1037,20 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1046,20 +1084,20 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1093,20 +1131,20 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1141,10 +1179,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1178,20 +1216,20 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1225,20 +1263,20 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1268,12 +1306,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.5" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1303,12 +1341,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1338,12 +1376,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1373,12 +1411,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1417,57 +1455,57 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="6" t="s">
-        <v>38</v>
+      <c r="A6" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1514,16 +1552,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1566,16 +1604,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1618,16 +1656,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1643,7 +1681,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1671,16 +1709,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1696,7 +1734,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
@@ -1714,10 +1754,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>46</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1733,7 +1773,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
@@ -1751,10 +1793,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>48</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>